<commit_message>
output: first scrapped data
</commit_message>
<xml_diff>
--- a/Base_Nom_Prenoms_ISE3_mission1.xlsx
+++ b/Base_Nom_Prenoms_ISE3_mission1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,36 +448,36 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Challengers</t>
+          <t>Furiosa - Une saga Mad Max</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>7.6</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>The Fall Guy</t>
+          <t>Civil War</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Civil War</t>
+          <t>Le Deuxième Acte</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>7.1</t>
+          <t>6.3</t>
         </is>
       </c>
     </row>
@@ -496,79 +496,79 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Comme un lundi</t>
+          <t>The Fall Guy</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6.3</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Jusqu’au bout du monde</t>
+          <t>Challengers</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>6.6</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Le mal n'existe pas</t>
+          <t>Atlas</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4.6</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Borgo</t>
+          <t>La Planète des singes - Le Nouveau Royaume</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6.4</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Border Line</t>
+          <t>Marcello Mio</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>6.8</t>
+          <t>5.6</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>L'Idée d'être avec toi</t>
+          <t>Comme un lundi</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>5.4</t>
+          <t>6.7</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Monkey Man</t>
+          <t>When Evil Lurks</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -580,103 +580,103 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>État limite</t>
+          <t>Les Trois Fantastiques</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>7.6</t>
+          <t>6.4</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Une affaire de principe</t>
+          <t>Borgo</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>6.6</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Le Tableau volé</t>
+          <t>Arthur the King</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>6.1</t>
+          <t>6.5</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Nous, les Leroy</t>
+          <t>South Park - La fin de l'obésité</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>6.6</t>
+          <t>7.1</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Back to Black</t>
+          <t>Jusqu’au bout du monde</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>6.5</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Frères</t>
+          <t>The Beekeeper</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>5.2</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Unfrosted - L'épopée de la Pop-Tart</t>
+          <t>L'Idée d'être avec toi</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4.4</t>
+          <t>5.2</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>LaRoy</t>
+          <t>Blue &amp; Compagnie</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>6.1</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>L'Homme aux mille visages</t>
+          <t>Border Line</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -688,67 +688,67 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Rebel Moon : Partie 2 - L'Entailleuse</t>
+          <t>Adagio</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Sky Dome 2123</t>
+          <t>Moi aussi</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>6.3</t>
+          <t>5.1</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>La Planète des singes - Le Nouveau Royaume</t>
+          <t>Monkey Man</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>6.8</t>
+          <t>6.5</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>S.O.S. Fantômes - La Menace de glace</t>
+          <t>Le Tableau volé</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>5.3</t>
+          <t>6.1</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Riddle of Fire</t>
+          <t>Mon oni à moi</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>6.9</t>
+          <t>5.9</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>L'Esprit Coubertin</t>
+          <t>Back to Black</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -760,120 +760,96 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Nicky Larson</t>
+          <t>Chien blanc</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>6.1</t>
+          <t>5.7</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Petites mains</t>
+          <t>Rebel Moon : Partie 2 - L'Entailleuse</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Les Cartes du mal</t>
+          <t>Les Intrus</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4.2</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Première affaire</t>
+          <t>Heroico</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5.4</t>
+          <t>6.5</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Blue &amp; Compagnie</t>
+          <t>Unfrosted - L'épopée de la Pop-Tart</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>4.5</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Baby Ruby</t>
+          <t>Baghead</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>4.9</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>The Greatest Hits</t>
+          <t>Baby Ruby</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5.4</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Baghead</t>
+          <t>La Mère de la mariée</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>5</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Puppy Love</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>5.3</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Les Vérités de Jennifer</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>5.8</t>
+          <t>4</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor: implement logging and restructure main function
</commit_message>
<xml_diff>
--- a/Base_Nom_Prenoms_ISE3_mission1.xlsx
+++ b/Base_Nom_Prenoms_ISE3_mission1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,90 +445,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Atlas</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>4.6</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Adagio</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Unfrosted - L'épopée de la Pop-Tart</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>4.6</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Arthur the King</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>6.6</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>La Mère de la mariée</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Mon oni à moi</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>5.8</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>South Park - La fin de l'obésité</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>7.2</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>